<commit_message>
Adicionando erro 90% e  estátistica descritiva no fomrato ideal para analise.
Apesar de no estudo todos os formatos de análise terem uso prático, a versão escolhida para ser mantida no Github será G1xG2xG3xM1xM2xM3 (Guidão1xGuidão2xGuidão3xMochila1xMochila2xMochila2). Além disso foram acrescentados o erro erro da frequência acumulada até 90% dos dados e a estatistica descritiva dos dados em "RESULTS".
</commit_message>
<xml_diff>
--- a/diferenca_altimetria_clean.xlsx
+++ b/diferenca_altimetria_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lobat\Documents\GitHub\Artigo-RTX-Moto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18DF0FE-4560-4F78-8432-74B84578750E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50754212-56A6-4098-A092-FFF2F228AD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{349D031E-3E46-41B2-B993-5E9D517FC08B}"/>
+    <workbookView xWindow="-20520" yWindow="2160" windowWidth="20640" windowHeight="11160" xr2:uid="{349D031E-3E46-41B2-B993-5E9D517FC08B}"/>
   </bookViews>
   <sheets>
     <sheet name="G1xG2xG3xM1xM2xM3" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NIV</t>
   </si>
@@ -41,10 +41,22 @@
     <t>PT</t>
   </si>
   <si>
-    <t>G</t>
+    <t>G1</t>
   </si>
   <si>
-    <t>M</t>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
   </si>
 </sst>
 </file>
@@ -370,9 +382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F4EE44-6091-4A63-88C2-C87744478CAA}">
   <dimension ref="A1:H990"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D2" sqref="D2"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -398,10 +410,18 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1">
       <c r="A2" s="6">
@@ -411,15 +431,23 @@
         <v>685.35749999999996</v>
       </c>
       <c r="C2" s="2">
-        <v>686.81859999999995</v>
+        <v>686.81299999999987</v>
       </c>
       <c r="D2" s="2">
-        <v>687.31190833333346</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="5"/>
+        <v>686.81319999999982</v>
+      </c>
+      <c r="E2" s="2">
+        <v>686.82959999999991</v>
+      </c>
+      <c r="F2" s="2">
+        <v>687.3128999999999</v>
+      </c>
+      <c r="G2" s="2">
+        <v>687.30072499999994</v>
+      </c>
+      <c r="H2" s="5">
+        <v>687.32210000000009</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1">
       <c r="A3" s="6">
@@ -429,15 +457,23 @@
         <v>685.3605</v>
       </c>
       <c r="C3" s="2">
-        <v>686.83293333333347</v>
+        <v>686.83079999999995</v>
       </c>
       <c r="D3" s="2">
-        <v>687.33059166666646</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="5"/>
+        <v>686.82690000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>686.8411000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>687.32619999999986</v>
+      </c>
+      <c r="G3" s="2">
+        <v>687.31927500000006</v>
+      </c>
+      <c r="H3" s="5">
+        <v>687.34629999999993</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1">
       <c r="A4" s="6">
@@ -447,15 +483,23 @@
         <v>685.37350000000004</v>
       </c>
       <c r="C4" s="2">
-        <v>686.84400000000005</v>
+        <v>686.83720000000005</v>
       </c>
       <c r="D4" s="2">
-        <v>687.33928333333336</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="5"/>
+        <v>686.83969999999999</v>
+      </c>
+      <c r="E4" s="2">
+        <v>686.85509999999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>687.33720000000017</v>
+      </c>
+      <c r="G4" s="2">
+        <v>687.33045000000016</v>
+      </c>
+      <c r="H4" s="5">
+        <v>687.35020000000009</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1">
       <c r="A5" s="6">
@@ -465,15 +509,23 @@
         <v>685.38149999999996</v>
       </c>
       <c r="C5" s="2">
-        <v>686.84956666666676</v>
+        <v>686.84360000000004</v>
       </c>
       <c r="D5" s="2">
-        <v>687.34803333333332</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="5"/>
+        <v>686.84500000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>686.8601000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>687.34809999999993</v>
+      </c>
+      <c r="G5" s="2">
+        <v>687.33870000000002</v>
+      </c>
+      <c r="H5" s="5">
+        <v>687.3572999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1">
       <c r="A6" s="6">
@@ -483,15 +535,23 @@
         <v>685.37800000000004</v>
       </c>
       <c r="C6" s="2">
-        <v>686.84906666666666</v>
+        <v>686.8429000000001</v>
       </c>
       <c r="D6" s="2">
-        <v>687.34627499999999</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="5"/>
+        <v>686.84640000000002</v>
+      </c>
+      <c r="E6" s="2">
+        <v>686.85790000000009</v>
+      </c>
+      <c r="F6" s="2">
+        <v>687.34349999999995</v>
+      </c>
+      <c r="G6" s="2">
+        <v>687.33922499999994</v>
+      </c>
+      <c r="H6" s="5">
+        <v>687.35610000000008</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1">
       <c r="A7" s="6">
@@ -501,15 +561,23 @@
         <v>685.37099999999998</v>
       </c>
       <c r="C7" s="2">
-        <v>686.84923333333336</v>
+        <v>686.84260000000006</v>
       </c>
       <c r="D7" s="2">
-        <v>687.34249166666666</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="5"/>
+        <v>686.84390000000008</v>
+      </c>
+      <c r="E7" s="2">
+        <v>686.86120000000005</v>
+      </c>
+      <c r="F7" s="2">
+        <v>687.34899999999993</v>
+      </c>
+      <c r="G7" s="2">
+        <v>687.33057500000007</v>
+      </c>
+      <c r="H7" s="5">
+        <v>687.34789999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1">
       <c r="A8" s="6">
@@ -519,15 +587,23 @@
         <v>685.37199999999996</v>
       </c>
       <c r="C8" s="2">
-        <v>686.85600000000011</v>
+        <v>686.85149999999999</v>
       </c>
       <c r="D8" s="2">
-        <v>687.34569999999997</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="5"/>
+        <v>686.85290000000009</v>
+      </c>
+      <c r="E8" s="2">
+        <v>686.86360000000002</v>
+      </c>
+      <c r="F8" s="2">
+        <v>687.34749999999997</v>
+      </c>
+      <c r="G8" s="2">
+        <v>687.3365</v>
+      </c>
+      <c r="H8" s="5">
+        <v>687.35310000000004</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1">
       <c r="A9" s="6">
@@ -537,15 +613,23 @@
         <v>685.39350000000002</v>
       </c>
       <c r="C9" s="2">
-        <v>686.86810000000014</v>
+        <v>686.86460000000011</v>
       </c>
       <c r="D9" s="2">
-        <v>687.36108333333334</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="5"/>
+        <v>686.86710000000005</v>
+      </c>
+      <c r="E9" s="2">
+        <v>686.87260000000003</v>
+      </c>
+      <c r="F9" s="2">
+        <v>687.36320000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>687.35425000000009</v>
+      </c>
+      <c r="H9" s="5">
+        <v>687.36579999999992</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1">
       <c r="A10" s="6">
@@ -555,15 +639,23 @@
         <v>685.41750000000002</v>
       </c>
       <c r="C10" s="2">
-        <v>686.88746666666668</v>
+        <v>686.88580000000002</v>
       </c>
       <c r="D10" s="2">
-        <v>687.38138333333336</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="5"/>
+        <v>686.8889999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>686.88760000000002</v>
+      </c>
+      <c r="F10" s="2">
+        <v>687.38550000000009</v>
+      </c>
+      <c r="G10" s="2">
+        <v>687.37555000000009</v>
+      </c>
+      <c r="H10" s="5">
+        <v>687.3830999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1">
       <c r="A11" s="6">
@@ -573,15 +665,23 @@
         <v>685.42700000000002</v>
       </c>
       <c r="C11" s="2">
-        <v>686.90336666666656</v>
+        <v>686.89959999999996</v>
       </c>
       <c r="D11" s="2">
-        <v>687.39556666666658</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
+        <v>686.90520000000004</v>
+      </c>
+      <c r="E11" s="2">
+        <v>686.90530000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>687.39409999999998</v>
+      </c>
+      <c r="G11" s="2">
+        <v>687.38819999999998</v>
+      </c>
+      <c r="H11" s="5">
+        <v>687.40440000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1">
       <c r="A12" s="6">
@@ -591,15 +691,23 @@
         <v>685.43349999999998</v>
       </c>
       <c r="C12" s="2">
-        <v>686.91346666666675</v>
+        <v>686.90710000000001</v>
       </c>
       <c r="D12" s="2">
-        <v>687.41094999999984</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="5"/>
+        <v>686.91430000000003</v>
+      </c>
+      <c r="E12" s="2">
+        <v>686.9190000000001</v>
+      </c>
+      <c r="F12" s="2">
+        <v>687.40819999999997</v>
+      </c>
+      <c r="G12" s="2">
+        <v>687.40124999999989</v>
+      </c>
+      <c r="H12" s="5">
+        <v>687.4233999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1">
       <c r="A13" s="6">
@@ -609,15 +717,23 @@
         <v>685.45050000000003</v>
       </c>
       <c r="C13" s="2">
-        <v>686.92759999999998</v>
+        <v>686.92100000000005</v>
       </c>
       <c r="D13" s="2">
-        <v>687.41768333333323</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="5"/>
+        <v>686.92920000000004</v>
+      </c>
+      <c r="E13" s="2">
+        <v>686.93259999999998</v>
+      </c>
+      <c r="F13" s="2">
+        <v>687.4156999999999</v>
+      </c>
+      <c r="G13" s="2">
+        <v>687.40774999999996</v>
+      </c>
+      <c r="H13" s="5">
+        <v>687.42960000000005</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1">
       <c r="A14" s="6">
@@ -627,15 +743,23 @@
         <v>685.45849999999996</v>
       </c>
       <c r="C14" s="2">
-        <v>686.93533333333335</v>
+        <v>686.92979999999989</v>
       </c>
       <c r="D14" s="2">
-        <v>687.42620833333331</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="5"/>
+        <v>686.93830000000003</v>
+      </c>
+      <c r="E14" s="2">
+        <v>686.93790000000013</v>
+      </c>
+      <c r="F14" s="2">
+        <v>687.42719999999997</v>
+      </c>
+      <c r="G14" s="2">
+        <v>687.4151250000001</v>
+      </c>
+      <c r="H14" s="5">
+        <v>687.43629999999996</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1">
       <c r="A15" s="6">
@@ -645,15 +769,23 @@
         <v>685.45749999999998</v>
       </c>
       <c r="C15" s="2">
-        <v>686.93793333333326</v>
+        <v>686.93360000000007</v>
       </c>
       <c r="D15" s="2">
-        <v>687.42558333333329</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="5"/>
+        <v>686.94089999999994</v>
+      </c>
+      <c r="E15" s="2">
+        <v>686.9393</v>
+      </c>
+      <c r="F15" s="2">
+        <v>687.41880000000003</v>
+      </c>
+      <c r="G15" s="2">
+        <v>687.41814999999997</v>
+      </c>
+      <c r="H15" s="5">
+        <v>687.43979999999988</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1">
       <c r="A16" s="6">
@@ -663,15 +795,23 @@
         <v>685.44550000000004</v>
       </c>
       <c r="C16" s="2">
-        <v>686.93066666666664</v>
+        <v>686.92609999999991</v>
       </c>
       <c r="D16" s="2">
-        <v>687.41869166666675</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="5"/>
+        <v>686.93409999999994</v>
+      </c>
+      <c r="E16" s="2">
+        <v>686.93179999999995</v>
+      </c>
+      <c r="F16" s="2">
+        <v>687.41930000000002</v>
+      </c>
+      <c r="G16" s="2">
+        <v>687.40917500000012</v>
+      </c>
+      <c r="H16" s="5">
+        <v>687.42759999999998</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="12.75" customHeight="1">
       <c r="A17" s="6">
@@ -681,15 +821,23 @@
         <v>685.44299999999998</v>
       </c>
       <c r="C17" s="2">
-        <v>686.92369999999994</v>
+        <v>686.92319999999995</v>
       </c>
       <c r="D17" s="2">
-        <v>687.40390833333333</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="5"/>
+        <v>686.92489999999998</v>
+      </c>
+      <c r="E17" s="2">
+        <v>686.923</v>
+      </c>
+      <c r="F17" s="2">
+        <v>687.40430000000003</v>
+      </c>
+      <c r="G17" s="2">
+        <v>687.39662500000009</v>
+      </c>
+      <c r="H17" s="5">
+        <v>687.41079999999999</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1">
       <c r="A18" s="6">
@@ -699,15 +847,23 @@
         <v>685.428</v>
       </c>
       <c r="C18" s="2">
-        <v>686.91693333333342</v>
+        <v>686.91340000000014</v>
       </c>
       <c r="D18" s="2">
-        <v>687.39822500000002</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="5"/>
+        <v>686.91910000000007</v>
+      </c>
+      <c r="E18" s="2">
+        <v>686.91830000000004</v>
+      </c>
+      <c r="F18" s="2">
+        <v>687.40190000000007</v>
+      </c>
+      <c r="G18" s="2">
+        <v>687.39037500000006</v>
+      </c>
+      <c r="H18" s="5">
+        <v>687.40240000000006</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="12.75" customHeight="1">
       <c r="A19" s="6">
@@ -717,15 +873,23 @@
         <v>685.447</v>
       </c>
       <c r="C19" s="2">
-        <v>686.92496666666682</v>
+        <v>686.92250000000001</v>
       </c>
       <c r="D19" s="2">
-        <v>687.40330833333337</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="5"/>
+        <v>686.9276000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>686.9248</v>
+      </c>
+      <c r="F19" s="2">
+        <v>687.40079999999989</v>
+      </c>
+      <c r="G19" s="2">
+        <v>687.397425</v>
+      </c>
+      <c r="H19" s="5">
+        <v>687.4117</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="12.75" customHeight="1">
       <c r="A20" s="6">
@@ -735,15 +899,23 @@
         <v>685.45150000000001</v>
       </c>
       <c r="C20" s="2">
-        <v>686.93639999999994</v>
+        <v>686.93240000000003</v>
       </c>
       <c r="D20" s="2">
-        <v>687.42449999999997</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="5"/>
+        <v>686.93929999999989</v>
+      </c>
+      <c r="E20" s="2">
+        <v>686.9375</v>
+      </c>
+      <c r="F20" s="2">
+        <v>687.42349999999999</v>
+      </c>
+      <c r="G20" s="2">
+        <v>687.42059999999992</v>
+      </c>
+      <c r="H20" s="5">
+        <v>687.42939999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1">
       <c r="A21" s="6">
@@ -753,15 +925,23 @@
         <v>685.47749999999996</v>
       </c>
       <c r="C21" s="2">
-        <v>686.95859999999993</v>
+        <v>686.95660000000009</v>
       </c>
       <c r="D21" s="2">
-        <v>687.44487500000014</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="5"/>
+        <v>686.95999999999992</v>
+      </c>
+      <c r="E21" s="2">
+        <v>686.95920000000001</v>
+      </c>
+      <c r="F21" s="2">
+        <v>687.44920000000002</v>
+      </c>
+      <c r="G21" s="2">
+        <v>687.43832500000008</v>
+      </c>
+      <c r="H21" s="5">
+        <v>687.44710000000009</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="12.75" customHeight="1">
       <c r="A22" s="6">
@@ -771,15 +951,23 @@
         <v>685.4905</v>
       </c>
       <c r="C22" s="2">
-        <v>686.9745999999999</v>
+        <v>686.96949999999993</v>
       </c>
       <c r="D22" s="2">
-        <v>687.45995833333336</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="5"/>
+        <v>686.9769</v>
+      </c>
+      <c r="E22" s="2">
+        <v>686.97739999999999</v>
+      </c>
+      <c r="F22" s="2">
+        <v>687.45249999999999</v>
+      </c>
+      <c r="G22" s="2">
+        <v>687.45387500000004</v>
+      </c>
+      <c r="H22" s="5">
+        <v>687.47350000000006</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1">
       <c r="A23" s="6">
@@ -789,15 +977,23 @@
         <v>685.49649999999997</v>
       </c>
       <c r="C23" s="2">
-        <v>686.98390000000006</v>
+        <v>686.97820000000013</v>
       </c>
       <c r="D23" s="2">
-        <v>687.47249166666677</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="5"/>
+        <v>686.98489999999993</v>
+      </c>
+      <c r="E23" s="2">
+        <v>686.98860000000002</v>
+      </c>
+      <c r="F23" s="2">
+        <v>687.4692</v>
+      </c>
+      <c r="G23" s="2">
+        <v>687.46267499999999</v>
+      </c>
+      <c r="H23" s="5">
+        <v>687.48559999999998</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1">
       <c r="A24" s="6">
@@ -807,15 +1003,23 @@
         <v>685.51499999999999</v>
       </c>
       <c r="C24" s="2">
-        <v>686.9928666666666</v>
+        <v>686.98799999999994</v>
       </c>
       <c r="D24" s="2">
-        <v>687.47794166666665</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="5"/>
+        <v>686.99329999999998</v>
+      </c>
+      <c r="E24" s="2">
+        <v>686.9973</v>
+      </c>
+      <c r="F24" s="2">
+        <v>687.47569999999996</v>
+      </c>
+      <c r="G24" s="2">
+        <v>687.47002499999996</v>
+      </c>
+      <c r="H24" s="5">
+        <v>687.48810000000014</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1">
       <c r="A25" s="6">
@@ -825,15 +1029,23 @@
         <v>685.51400000000001</v>
       </c>
       <c r="C25" s="2">
-        <v>686.99189999999999</v>
+        <v>686.98849999999993</v>
       </c>
       <c r="D25" s="2">
-        <v>687.48236666666662</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="5"/>
+        <v>686.99270000000001</v>
+      </c>
+      <c r="E25" s="2">
+        <v>686.9944999999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>687.48289999999997</v>
+      </c>
+      <c r="G25" s="2">
+        <v>687.47559999999999</v>
+      </c>
+      <c r="H25" s="5">
+        <v>687.48860000000002</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1">
       <c r="A26" s="6">
@@ -843,15 +1055,23 @@
         <v>685.505</v>
       </c>
       <c r="C26" s="2">
-        <v>686.98566666666659</v>
+        <v>686.9833000000001</v>
       </c>
       <c r="D26" s="2">
-        <v>687.47073333333321</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="5"/>
+        <v>686.98879999999997</v>
+      </c>
+      <c r="E26" s="2">
+        <v>686.98490000000004</v>
+      </c>
+      <c r="F26" s="2">
+        <v>687.46879999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>687.46420000000012</v>
+      </c>
+      <c r="H26" s="5">
+        <v>687.47919999999999</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1">
       <c r="A27" s="6">
@@ -861,15 +1081,23 @@
         <v>685.48249999999996</v>
       </c>
       <c r="C27" s="2">
-        <v>686.97220000000004</v>
+        <v>686.96989999999994</v>
       </c>
       <c r="D27" s="2">
-        <v>687.45575833333339</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="5"/>
+        <v>686.97530000000006</v>
+      </c>
+      <c r="E27" s="2">
+        <v>686.97140000000002</v>
+      </c>
+      <c r="F27" s="2">
+        <v>687.45619999999997</v>
+      </c>
+      <c r="G27" s="2">
+        <v>687.44797500000004</v>
+      </c>
+      <c r="H27" s="5">
+        <v>687.46310000000005</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1">
       <c r="A28" s="6">
@@ -879,15 +1107,23 @@
         <v>685.47400000000005</v>
       </c>
       <c r="C28" s="2">
-        <v>686.96316666666655</v>
+        <v>686.96060000000011</v>
       </c>
       <c r="D28" s="2">
-        <v>687.44203333333337</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="5"/>
+        <v>686.96629999999993</v>
+      </c>
+      <c r="E28" s="2">
+        <v>686.96259999999995</v>
+      </c>
+      <c r="F28" s="2">
+        <v>687.43979999999999</v>
+      </c>
+      <c r="G28" s="2">
+        <v>687.43630000000007</v>
+      </c>
+      <c r="H28" s="5">
+        <v>687.45</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1">
       <c r="A29" s="6">
@@ -897,15 +1133,23 @@
         <v>685.46799999999996</v>
       </c>
       <c r="C29" s="2">
-        <v>686.9608333333332</v>
+        <v>686.95669999999996</v>
       </c>
       <c r="D29" s="2">
-        <v>687.44009999999992</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="5"/>
+        <v>686.96660000000008</v>
+      </c>
+      <c r="E29" s="2">
+        <v>686.95920000000001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>687.43939999999998</v>
+      </c>
+      <c r="G29" s="2">
+        <v>687.43290000000002</v>
+      </c>
+      <c r="H29" s="5">
+        <v>687.44799999999998</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="12.75" customHeight="1">
       <c r="A30" s="6">
@@ -915,15 +1159,23 @@
         <v>685.47950000000003</v>
       </c>
       <c r="C30" s="2">
-        <v>686.96556666666663</v>
+        <v>686.96229999999991</v>
       </c>
       <c r="D30" s="2">
-        <v>687.44881666666663</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="5"/>
+        <v>686.97059999999988</v>
+      </c>
+      <c r="E30" s="2">
+        <v>686.96379999999988</v>
+      </c>
+      <c r="F30" s="2">
+        <v>687.44979999999998</v>
+      </c>
+      <c r="G30" s="2">
+        <v>687.44145000000003</v>
+      </c>
+      <c r="H30" s="5">
+        <v>687.45519999999999</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="12.75" customHeight="1">
       <c r="A31" s="6">
@@ -933,15 +1185,23 @@
         <v>685.49350000000004</v>
       </c>
       <c r="C31" s="2">
-        <v>686.97783333333336</v>
+        <v>686.97450000000003</v>
       </c>
       <c r="D31" s="2">
-        <v>687.45698333333337</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="5"/>
+        <v>686.9846</v>
+      </c>
+      <c r="E31" s="2">
+        <v>686.97439999999995</v>
+      </c>
+      <c r="F31" s="2">
+        <v>687.45799999999997</v>
+      </c>
+      <c r="G31" s="2">
+        <v>687.44994999999994</v>
+      </c>
+      <c r="H31" s="5">
+        <v>687.46300000000008</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="12.75" customHeight="1">
       <c r="A32" s="6">
@@ -951,15 +1211,23 @@
         <v>685.49249999999995</v>
       </c>
       <c r="C32" s="2">
-        <v>686.98623333333342</v>
+        <v>686.98220000000003</v>
       </c>
       <c r="D32" s="2">
-        <v>687.47117500000002</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="5"/>
+        <v>686.9905</v>
+      </c>
+      <c r="E32" s="2">
+        <v>686.9860000000001</v>
+      </c>
+      <c r="F32" s="2">
+        <v>687.47770000000003</v>
+      </c>
+      <c r="G32" s="2">
+        <v>687.45802500000002</v>
+      </c>
+      <c r="H32" s="5">
+        <v>687.4778</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="12.75" customHeight="1">
       <c r="A33" s="6">
@@ -969,15 +1237,23 @@
         <v>685.51250000000005</v>
       </c>
       <c r="C33" s="2">
-        <v>687.00223333333327</v>
+        <v>687.00299999999993</v>
       </c>
       <c r="D33" s="2">
-        <v>687.4828083333332</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="5"/>
+        <v>687.00440000000003</v>
+      </c>
+      <c r="E33" s="2">
+        <v>686.99930000000006</v>
+      </c>
+      <c r="F33" s="2">
+        <v>687.47759999999994</v>
+      </c>
+      <c r="G33" s="2">
+        <v>687.47622499999989</v>
+      </c>
+      <c r="H33" s="5">
+        <v>687.49459999999999</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="12.75" customHeight="1">
       <c r="A34" s="6">
@@ -987,15 +1263,23 @@
         <v>685.52</v>
       </c>
       <c r="C34" s="2">
-        <v>687.01536666666664</v>
+        <v>687.01340000000005</v>
       </c>
       <c r="D34" s="2">
-        <v>687.50008333333335</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="5"/>
+        <v>687.01949999999988</v>
+      </c>
+      <c r="E34" s="2">
+        <v>687.0132000000001</v>
+      </c>
+      <c r="F34" s="2">
+        <v>687.50490000000002</v>
+      </c>
+      <c r="G34" s="2">
+        <v>687.48835000000008</v>
+      </c>
+      <c r="H34" s="5">
+        <v>687.50700000000006</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1">
       <c r="A35" s="6">
@@ -1005,15 +1289,23 @@
         <v>685.53599999999994</v>
       </c>
       <c r="C35" s="2">
-        <v>687.02756666666664</v>
+        <v>687.02790000000005</v>
       </c>
       <c r="D35" s="2">
-        <v>687.51592500000004</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="5"/>
+        <v>687.03039999999999</v>
+      </c>
+      <c r="E35" s="2">
+        <v>687.0243999999999</v>
+      </c>
+      <c r="F35" s="2">
+        <v>687.51930000000004</v>
+      </c>
+      <c r="G35" s="2">
+        <v>687.5060749999999</v>
+      </c>
+      <c r="H35" s="5">
+        <v>687.52240000000006</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="12.75" customHeight="1">
       <c r="A36" s="6">
@@ -1023,15 +1315,23 @@
         <v>685.55</v>
       </c>
       <c r="C36" s="2">
-        <v>687.0413666666667</v>
+        <v>687.04269999999997</v>
       </c>
       <c r="D36" s="2">
-        <v>687.53183333333334</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="5"/>
+        <v>687.04499999999985</v>
+      </c>
+      <c r="E36" s="2">
+        <v>687.03639999999996</v>
+      </c>
+      <c r="F36" s="2">
+        <v>687.53359999999998</v>
+      </c>
+      <c r="G36" s="2">
+        <v>687.52170000000001</v>
+      </c>
+      <c r="H36" s="5">
+        <v>687.54020000000003</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1">
       <c r="A37" s="6">
@@ -1041,15 +1341,23 @@
         <v>685.56399999999996</v>
       </c>
       <c r="C37" s="2">
-        <v>687.05333333333328</v>
+        <v>687.05349999999987</v>
       </c>
       <c r="D37" s="2">
-        <v>687.54259166666668</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="5"/>
+        <v>687.05640000000017</v>
+      </c>
+      <c r="E37" s="2">
+        <v>687.05010000000004</v>
+      </c>
+      <c r="F37" s="2">
+        <v>687.54130000000009</v>
+      </c>
+      <c r="G37" s="2">
+        <v>687.53487500000006</v>
+      </c>
+      <c r="H37" s="5">
+        <v>687.55160000000001</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1">
       <c r="A38" s="6">
@@ -1059,15 +1367,23 @@
         <v>685.57449999999994</v>
       </c>
       <c r="C38" s="2">
-        <v>687.05723333333333</v>
+        <v>687.05500000000006</v>
       </c>
       <c r="D38" s="2">
-        <v>687.55347500000005</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="5"/>
+        <v>687.06000000000006</v>
+      </c>
+      <c r="E38" s="2">
+        <v>687.05669999999986</v>
+      </c>
+      <c r="F38" s="2">
+        <v>687.5553000000001</v>
+      </c>
+      <c r="G38" s="2">
+        <v>687.54362500000002</v>
+      </c>
+      <c r="H38" s="5">
+        <v>687.56150000000002</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1">
       <c r="A39" s="6">
@@ -1077,15 +1393,23 @@
         <v>685.57749999999999</v>
       </c>
       <c r="C39" s="2">
-        <v>687.06260000000009</v>
+        <v>687.06060000000002</v>
       </c>
       <c r="D39" s="2">
-        <v>687.55612499999995</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="5"/>
+        <v>687.06610000000001</v>
+      </c>
+      <c r="E39" s="2">
+        <v>687.06110000000012</v>
+      </c>
+      <c r="F39" s="2">
+        <v>687.5560999999999</v>
+      </c>
+      <c r="G39" s="2">
+        <v>687.54597499999988</v>
+      </c>
+      <c r="H39" s="5">
+        <v>687.56629999999996</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1">
       <c r="A40" s="6">
@@ -1095,15 +1419,23 @@
         <v>685.57899999999995</v>
       </c>
       <c r="C40" s="2">
-        <v>687.05859999999996</v>
+        <v>687.0571000000001</v>
       </c>
       <c r="D40" s="2">
-        <v>687.55363333333344</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="5"/>
+        <v>687.06200000000013</v>
+      </c>
+      <c r="E40" s="2">
+        <v>687.05669999999986</v>
+      </c>
+      <c r="F40" s="2">
+        <v>687.55420000000015</v>
+      </c>
+      <c r="G40" s="2">
+        <v>687.54510000000005</v>
+      </c>
+      <c r="H40" s="5">
+        <v>687.5616</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1">
       <c r="A41" s="6">
@@ -1113,15 +1445,23 @@
         <v>685.57349999999997</v>
       </c>
       <c r="C41" s="2">
-        <v>687.05126666666672</v>
+        <v>687.04910000000007</v>
       </c>
       <c r="D41" s="2">
-        <v>687.5398583333332</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="5"/>
+        <v>687.05560000000003</v>
+      </c>
+      <c r="E41" s="2">
+        <v>687.04909999999995</v>
+      </c>
+      <c r="F41" s="2">
+        <v>687.54179999999997</v>
+      </c>
+      <c r="G41" s="2">
+        <v>687.530575</v>
+      </c>
+      <c r="H41" s="5">
+        <v>687.54719999999998</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1">
       <c r="A42" s="6">
@@ -1131,15 +1471,23 @@
         <v>685.5625</v>
       </c>
       <c r="C42" s="2">
-        <v>687.03903333333312</v>
+        <v>687.03709999999978</v>
       </c>
       <c r="D42" s="2">
-        <v>687.52994999999999</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="5"/>
+        <v>687.04409999999996</v>
+      </c>
+      <c r="E42" s="2">
+        <v>687.03590000000008</v>
+      </c>
+      <c r="F42" s="2">
+        <v>687.5329999999999</v>
+      </c>
+      <c r="G42" s="2">
+        <v>687.52074999999991</v>
+      </c>
+      <c r="H42" s="5">
+        <v>687.53610000000003</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1">
       <c r="A43" s="6">
@@ -1149,15 +1497,23 @@
         <v>685.54849999999999</v>
       </c>
       <c r="C43" s="2">
-        <v>687.03593333333322</v>
+        <v>687.03290000000004</v>
       </c>
       <c r="D43" s="2">
-        <v>687.51679166666656</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="5"/>
+        <v>687.04310000000009</v>
+      </c>
+      <c r="E43" s="2">
+        <v>687.03179999999998</v>
+      </c>
+      <c r="F43" s="2">
+        <v>687.52170000000001</v>
+      </c>
+      <c r="G43" s="2">
+        <v>687.50727499999994</v>
+      </c>
+      <c r="H43" s="5">
+        <v>687.52139999999997</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1">
       <c r="A44" s="6">
@@ -1167,15 +1523,23 @@
         <v>685.54750000000001</v>
       </c>
       <c r="C44" s="2">
-        <v>687.03463333333332</v>
+        <v>687.02980000000002</v>
       </c>
       <c r="D44" s="2">
-        <v>687.51591666666673</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="5"/>
+        <v>687.04150000000004</v>
+      </c>
+      <c r="E44" s="2">
+        <v>687.0326</v>
+      </c>
+      <c r="F44" s="2">
+        <v>687.52320000000009</v>
+      </c>
+      <c r="G44" s="2">
+        <v>687.50515000000007</v>
+      </c>
+      <c r="H44" s="5">
+        <v>687.51940000000002</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="12.75" customHeight="1">
       <c r="A45" s="6">
@@ -1185,15 +1549,23 @@
         <v>685.54700000000003</v>
       </c>
       <c r="C45" s="2">
-        <v>687.03710000000001</v>
+        <v>687.03189999999995</v>
       </c>
       <c r="D45" s="2">
-        <v>687.52074166666659</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="5"/>
+        <v>687.04499999999996</v>
+      </c>
+      <c r="E45" s="2">
+        <v>687.03439999999989</v>
+      </c>
+      <c r="F45" s="2">
+        <v>687.5184999999999</v>
+      </c>
+      <c r="G45" s="2">
+        <v>687.51322499999992</v>
+      </c>
+      <c r="H45" s="5">
+        <v>687.53050000000007</v>
+      </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1">
       <c r="A46" s="6">
@@ -1203,15 +1575,23 @@
         <v>685.55600000000004</v>
       </c>
       <c r="C46" s="2">
-        <v>687.04439999999988</v>
+        <v>687.03779999999995</v>
       </c>
       <c r="D46" s="2">
-        <v>687.52737500000001</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="5"/>
+        <v>687.05089999999996</v>
+      </c>
+      <c r="E46" s="2">
+        <v>687.04450000000008</v>
+      </c>
+      <c r="F46" s="2">
+        <v>687.53180000000009</v>
+      </c>
+      <c r="G46" s="2">
+        <v>687.51582499999995</v>
+      </c>
+      <c r="H46" s="5">
+        <v>687.53449999999998</v>
+      </c>
     </row>
     <row r="47" spans="1:8" ht="12.75" customHeight="1">
       <c r="A47" s="6">
@@ -1221,15 +1601,23 @@
         <v>685.56399999999996</v>
       </c>
       <c r="C47" s="2">
-        <v>687.05223333333345</v>
+        <v>687.04729999999995</v>
       </c>
       <c r="D47" s="2">
-        <v>687.53546666666659</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="5"/>
+        <v>687.05800000000022</v>
+      </c>
+      <c r="E47" s="2">
+        <v>687.05140000000006</v>
+      </c>
+      <c r="F47" s="2">
+        <v>687.53419999999983</v>
+      </c>
+      <c r="G47" s="2">
+        <v>687.52840000000003</v>
+      </c>
+      <c r="H47" s="5">
+        <v>687.54380000000003</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="12.75" customHeight="1">
       <c r="A48" s="6">
@@ -1239,15 +1627,23 @@
         <v>685.5675</v>
       </c>
       <c r="C48" s="2">
-        <v>687.05690000000004</v>
+        <v>687.05080000000009</v>
       </c>
       <c r="D48" s="2">
-        <v>687.54140833333338</v>
-      </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="5"/>
+        <v>687.06220000000008</v>
+      </c>
+      <c r="E48" s="2">
+        <v>687.05769999999995</v>
+      </c>
+      <c r="F48" s="2">
+        <v>687.53989999999999</v>
+      </c>
+      <c r="G48" s="2">
+        <v>687.5341249999999</v>
+      </c>
+      <c r="H48" s="5">
+        <v>687.55020000000013</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="12.75" customHeight="1">
       <c r="A49" s="6">
@@ -1257,15 +1653,23 @@
         <v>685.57500000000005</v>
       </c>
       <c r="C49" s="2">
-        <v>687.06550000000004</v>
+        <v>687.06090000000006</v>
       </c>
       <c r="D49" s="2">
-        <v>687.54427499999986</v>
-      </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="5"/>
+        <v>687.06999999999994</v>
+      </c>
+      <c r="E49" s="2">
+        <v>687.0655999999999</v>
+      </c>
+      <c r="F49" s="2">
+        <v>687.54589999999996</v>
+      </c>
+      <c r="G49" s="2">
+        <v>687.53572499999996</v>
+      </c>
+      <c r="H49" s="5">
+        <v>687.55120000000011</v>
+      </c>
     </row>
     <row r="50" spans="1:8" ht="12.75" customHeight="1">
       <c r="A50" s="6">
@@ -1275,15 +1679,23 @@
         <v>685.57950000000005</v>
       </c>
       <c r="C50" s="2">
+        <v>687.06570000000011</v>
+      </c>
+      <c r="D50" s="2">
+        <v>687.07550000000015</v>
+      </c>
+      <c r="E50" s="2">
         <v>687.07060000000001</v>
       </c>
-      <c r="D50" s="2">
-        <v>687.55365000000018</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="5"/>
+      <c r="F50" s="2">
+        <v>687.55269999999996</v>
+      </c>
+      <c r="G50" s="2">
+        <v>687.54785000000004</v>
+      </c>
+      <c r="H50" s="5">
+        <v>687.56040000000007</v>
+      </c>
     </row>
     <row r="51" spans="1:8" ht="12.75" customHeight="1">
       <c r="A51" s="6">
@@ -1293,15 +1705,23 @@
         <v>685.60050000000001</v>
       </c>
       <c r="C51" s="2">
+        <v>687.0784000000001</v>
+      </c>
+      <c r="D51" s="2">
+        <v>687.0874</v>
+      </c>
+      <c r="E51" s="2">
         <v>687.0829</v>
       </c>
-      <c r="D51" s="2">
-        <v>687.56700833333343</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="5"/>
+      <c r="F51" s="2">
+        <v>687.57339999999999</v>
+      </c>
+      <c r="G51" s="2">
+        <v>687.55962499999998</v>
+      </c>
+      <c r="H51" s="5">
+        <v>687.5680000000001</v>
+      </c>
     </row>
     <row r="52" spans="1:8" ht="12.75" customHeight="1">
       <c r="A52" s="6">
@@ -1311,15 +1731,23 @@
         <v>685.62450000000001</v>
       </c>
       <c r="C52" s="2">
-        <v>687.09413333333339</v>
+        <v>687.08960000000002</v>
       </c>
       <c r="D52" s="2">
-        <v>687.57909166666684</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="5"/>
+        <v>687.09820000000002</v>
+      </c>
+      <c r="E52" s="2">
+        <v>687.09460000000013</v>
+      </c>
+      <c r="F52" s="2">
+        <v>687.58029999999997</v>
+      </c>
+      <c r="G52" s="2">
+        <v>687.57297500000004</v>
+      </c>
+      <c r="H52" s="5">
+        <v>687.58400000000006</v>
+      </c>
     </row>
     <row r="53" spans="1:8" ht="12.75" customHeight="1">
       <c r="A53" s="1"/>

</xml_diff>